<commit_message>
added column "team0_starting_side" in table "Matches"
</commit_message>
<xml_diff>
--- a/docs/Datenbankstruktur.xlsx
+++ b/docs/Datenbankstruktur.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CompTracker\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CompTracker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F336AA8-E284-49EB-8D4B-F402379E4AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B524EB7-3209-4528-830A-8823C943BD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A43C1E1-4ABB-41E7-9B44-348B4524206A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A43C1E1-4ABB-41E7-9B44-348B4524206A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>Matches</t>
   </si>
@@ -321,6 +321,21 @@
   </si>
   <si>
     <t>time/plant/kill</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>prep/round/plant</t>
+  </si>
+  <si>
+    <t>atk lost rounds</t>
+  </si>
+  <si>
+    <t>def lost rounds</t>
+  </si>
+  <si>
+    <t>Team 0 starting side</t>
   </si>
 </sst>
 </file>
@@ -706,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71C096D-CD28-4CC0-BEF1-D1B9E98FC535}">
   <dimension ref="B1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,6 +754,9 @@
       <c r="C2" t="s">
         <v>77</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
@@ -751,9 +769,6 @@
       <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
-        <v>5</v>
-      </c>
       <c r="L2" t="s">
         <v>6</v>
       </c>
@@ -762,6 +777,9 @@
       </c>
       <c r="N2" t="s">
         <v>17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
@@ -947,6 +965,12 @@
       <c r="S10" t="s">
         <v>88</v>
       </c>
+      <c r="T10" t="s">
+        <v>97</v>
+      </c>
+      <c r="U10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -975,6 +999,14 @@
       </c>
       <c r="J12" t="s">
         <v>82</v>
+      </c>
+      <c r="K12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated database structure in docs
</commit_message>
<xml_diff>
--- a/docs/Datenbankstruktur.xlsx
+++ b/docs/Datenbankstruktur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CompTracker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B524EB7-3209-4528-830A-8823C943BD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17A31FF-E90D-4BE2-9929-85D5DA574FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A43C1E1-4ABB-41E7-9B44-348B4524206A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A43C1E1-4ABB-41E7-9B44-348B4524206A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
   <si>
     <t>Matches</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>Team 0 starting side</t>
+  </si>
+  <si>
+    <t>got_refrafgt</t>
   </si>
 </sst>
 </file>
@@ -719,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71C096D-CD28-4CC0-BEF1-D1B9E98FC535}">
-  <dimension ref="B1:W31"/>
+  <dimension ref="B1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,9 +879,6 @@
       <c r="K8" t="s">
         <v>21</v>
       </c>
-      <c r="L8" t="s">
-        <v>22</v>
-      </c>
       <c r="M8" t="s">
         <v>23</v>
       </c>
@@ -1003,6 +1003,9 @@
       <c r="K12" t="s">
         <v>95</v>
       </c>
+      <c r="L12" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
@@ -1163,6 +1166,111 @@
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1170,5 +1278,6 @@
     <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated databse structure for player_matches table [+ods_atk, +oks_atk]
implemented extract_player_match_data in extractData.py
</commit_message>
<xml_diff>
--- a/docs/Datenbankstruktur.xlsx
+++ b/docs/Datenbankstruktur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CompTracker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17A31FF-E90D-4BE2-9929-85D5DA574FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC1325A-1BD5-494F-8FEB-995BDAFFF796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A43C1E1-4ABB-41E7-9B44-348B4524206A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
   <si>
     <t>Matches</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>got_refrafgt</t>
+  </si>
+  <si>
+    <t>oks_atk</t>
+  </si>
+  <si>
+    <t>ods_atk</t>
   </si>
 </sst>
 </file>
@@ -722,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71C096D-CD28-4CC0-BEF1-D1B9E98FC535}">
-  <dimension ref="B1:W54"/>
+  <dimension ref="B1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,6 +977,12 @@
       <c r="U10" t="s">
         <v>98</v>
       </c>
+      <c r="V10" t="s">
+        <v>101</v>
+      </c>
+      <c r="W10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1169,109 +1181,10 @@
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>23</v>
-      </c>
+      <c r="C34" s="1"/>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>84</v>
-      </c>
+      <c r="C45" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updated database_structure for matches table [+prep_duration,+round_duration,+plant_duration] and player_match table [+refrags,+got_refragged]
implemented it also in extractData.py
</commit_message>
<xml_diff>
--- a/docs/Datenbankstruktur.xlsx
+++ b/docs/Datenbankstruktur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CompTracker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC1325A-1BD5-494F-8FEB-995BDAFFF796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3119B0-A6BC-4E6C-AA0F-76D336C5EBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A43C1E1-4ABB-41E7-9B44-348B4524206A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
   <si>
     <t>Matches</t>
   </si>
@@ -345,6 +345,18 @@
   </si>
   <si>
     <t>ods_atk</t>
+  </si>
+  <si>
+    <t>prep_duration</t>
+  </si>
+  <si>
+    <t>round_duration</t>
+  </si>
+  <si>
+    <t>plant_duration</t>
+  </si>
+  <si>
+    <t>gor_refragged</t>
   </si>
 </sst>
 </file>
@@ -728,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71C096D-CD28-4CC0-BEF1-D1B9E98FC535}">
-  <dimension ref="B1:W45"/>
+  <dimension ref="B1:Y45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +758,7 @@
     <col min="16" max="17" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
@@ -756,7 +768,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,8 +802,17 @@
       <c r="O2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>104</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -811,7 +832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -852,12 +873,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="P7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
@@ -919,7 +940,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -983,8 +1004,14 @@
       <c r="W10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="X10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1019,12 +1046,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -1032,7 +1059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1043,7 +1070,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>40</v>
       </c>

</xml_diff>